<commit_message>
excel create row cell
</commit_message>
<xml_diff>
--- a/doc/test1.xlsx
+++ b/doc/test1.xlsx
@@ -56,13 +56,16 @@
     <definedName name="s19b">Sheet2!$D$7</definedName>
     <definedName name="s19c">Sheet2!$E$7</definedName>
     <definedName name="s19d">Sheet2!$F$7</definedName>
+    <definedName name="hbtest">Sheet1!$N$4:$O$5</definedName>
+    <definedName name="listTest">Sheet1!$D$34</definedName>
+    <definedName name="listList">Sheet1!$F$34</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>报告编号：</t>
   </si>
@@ -193,6 +196,18 @@
     </r>
   </si>
   <si>
+    <t>图书</t>
+  </si>
+  <si>
+    <t>家居厨具</t>
+  </si>
+  <si>
+    <t>东北</t>
+  </si>
+  <si>
+    <t>华北</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -213,6 +228,9 @@
     </r>
   </si>
   <si>
+    <t>华东</t>
+  </si>
+  <si>
     <t>{fxpj}</t>
   </si>
   <si>
@@ -308,6 +326,12 @@
     <t xml:space="preserve">  近12个月中开票总金额：</t>
   </si>
   <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>listList</t>
+  </si>
+  <si>
     <t>第1季度增值税纳税额</t>
   </si>
   <si>
@@ -346,12 +370,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ \¥* #,##0.00_ ;_ \¥* \-#,##0.00_ ;_ \¥* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ \¥* #,##0_ ;_ \¥* \-#,##0_ ;_ \¥* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="_ \¥* #,##0.00_ ;_ \¥* \-#,##0.00_ ;_ \¥* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ \¥* #,##0_ ;_ \¥* \-#,##0_ ;_ \¥* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -400,6 +424,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF6A8759"/>
+      <name val="Consolas"/>
       <charset val="134"/>
     </font>
     <font>
@@ -573,187 +603,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFCCC0DA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6B8B7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB8CCE4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8E4BC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8064A2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4F81BD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC0504D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BBB59"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95B3D7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC4D79B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDA9694"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFABF8F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB1A0C7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE4DFEC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2DCDB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDE9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDAEEF3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4BACC6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFB7DEE8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFCCC0DA"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6B8B7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB8CCE4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FF92CDDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF79646"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCD5B4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD8E4BC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4BACC6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8064A2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4F81BD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC0504D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF79646"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9BBB59"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFABF8F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB1A0C7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF95B3D7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC4D79B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFDE9D9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEBF1DE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92CDDC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDA9694"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE4DFEC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2DCDB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDCE6F1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDAEEF3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -887,10 +917,10 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -899,137 +929,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1084,13 +1114,22 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1152,6 +1191,808 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0946346873700263"/>
+          <c:y val="0.228468899521531"/>
+          <c:w val="0.901206155552475"/>
+          <c:h val="0.701291866028708"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$18:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="317710095"/>
+        <c:axId val="346245557"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="317710095"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="346245557"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="346245557"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="317710095"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1220,6 +2061,36 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>490855</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>158115</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>408940</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>69215</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="8175625" y="2939415"/>
+        <a:ext cx="4572000" cy="2743200"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1486,10 +2357,10 @@
     <outlinePr showOutlineSymbols="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="B1:K26"/>
+  <dimension ref="B1:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5"/>
@@ -1545,7 +2416,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" ht="27" customHeight="1" spans="2:11">
+    <row r="4" ht="27" customHeight="1" spans="2:15">
       <c r="B4" s="2"/>
       <c r="C4" s="5" t="s">
         <v>2</v>
@@ -1558,8 +2429,10 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="2"/>
-    </row>
-    <row r="5" ht="16.5" spans="2:11">
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+    </row>
+    <row r="5" ht="16.5" spans="2:15">
       <c r="B5" s="2"/>
       <c r="C5" s="7" t="s">
         <v>3</v>
@@ -1574,6 +2447,8 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="2"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
     </row>
     <row r="6" ht="16.5" spans="2:11">
       <c r="B6" s="2"/>
@@ -1591,7 +2466,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" ht="16.5" spans="2:11">
+    <row r="7" ht="16.5" spans="2:21">
       <c r="B7" s="2"/>
       <c r="C7" s="7" t="s">
         <v>7</v>
@@ -1606,8 +2481,14 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" ht="16.5" spans="2:11">
+      <c r="T7" t="s">
+        <v>9</v>
+      </c>
+      <c r="U7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" ht="16.5" spans="2:21">
       <c r="B8" s="2"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -1618,8 +2499,17 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" ht="9" customHeight="1" spans="2:11">
+      <c r="S8" t="s">
+        <v>11</v>
+      </c>
+      <c r="T8">
+        <v>2522</v>
+      </c>
+      <c r="U8">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="9" ht="9" customHeight="1" spans="2:21">
       <c r="B9" s="2"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -1630,11 +2520,20 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" ht="21" customHeight="1" spans="2:11">
+      <c r="S9" t="s">
+        <v>12</v>
+      </c>
+      <c r="T9">
+        <v>156</v>
+      </c>
+      <c r="U9">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="10" ht="21" customHeight="1" spans="2:21">
       <c r="B10" s="2"/>
       <c r="C10" s="5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1644,19 +2543,28 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
       <c r="K10" s="2"/>
+      <c r="S10" t="s">
+        <v>14</v>
+      </c>
+      <c r="T10">
+        <v>1566</v>
+      </c>
+      <c r="U10">
+        <v>3031</v>
+      </c>
     </row>
     <row r="11" ht="16.5" spans="2:11">
       <c r="B11" s="2"/>
       <c r="C11" s="7"/>
       <c r="D11" s="10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -1669,10 +2577,10 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -1682,16 +2590,16 @@
     <row r="13" ht="16.5" spans="2:11">
       <c r="B13" s="2"/>
       <c r="D13" s="10" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J13">
         <f>SUM(J17,J18)</f>
@@ -1726,7 +2634,7 @@
     <row r="16" ht="25" customHeight="1" spans="2:11">
       <c r="B16" s="2"/>
       <c r="C16" s="5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -1740,17 +2648,17 @@
     <row r="17" ht="16.5" spans="2:11">
       <c r="B17" s="2"/>
       <c r="C17" s="16" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="18">
+      <c r="J17" s="21">
         <f>SUM(Sheet2!C7:F7)</f>
         <v>0</v>
       </c>
@@ -1759,17 +2667,17 @@
     <row r="18" ht="16.5" spans="2:11">
       <c r="B18" s="2"/>
       <c r="C18" s="7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="J18" s="19">
+      <c r="J18" s="22">
         <f>SUM(Sheet2!C5:F7)</f>
         <v>40</v>
       </c>
@@ -1778,17 +2686,17 @@
     <row r="19" ht="16.5" spans="2:11">
       <c r="B19" s="2"/>
       <c r="C19" s="7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="20" t="e">
+      <c r="J19" s="23" t="e">
         <f>(SUM(Sheet2!C7:F7)/SUM(Sheet2!C6:F7))*100%</f>
         <v>#DIV/0!</v>
       </c>
@@ -1797,13 +2705,13 @@
     <row r="20" ht="16.5" spans="2:11">
       <c r="B20" s="2"/>
       <c r="C20" s="7" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
@@ -1813,13 +2721,13 @@
     <row r="21" ht="16.5" spans="2:11">
       <c r="B21" s="2"/>
       <c r="C21" s="7" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -1829,13 +2737,13 @@
     <row r="22" ht="16.5" spans="2:11">
       <c r="B22" s="2"/>
       <c r="C22" s="7" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
@@ -1845,13 +2753,13 @@
     <row r="23" ht="16.5" spans="2:11">
       <c r="B23" s="2"/>
       <c r="C23" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
@@ -1861,13 +2769,13 @@
     <row r="24" ht="16.5" spans="2:11">
       <c r="B24" s="2"/>
       <c r="C24" s="7" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -1898,9 +2806,21 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
+    <row r="33" ht="18" spans="4:6">
+      <c r="D33" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4">
+      <c r="D34" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C8:F8"/>
+    <mergeCell ref="N4:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1926,21 +2846,21 @@
     <row r="4" spans="2:6">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1">
         <v>10</v>
@@ -1957,7 +2877,7 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -1966,7 +2886,7 @@
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1976,21 +2896,21 @@
     <row r="12" spans="2:6">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C13" s="1">
         <v>120000</v>
@@ -2007,7 +2927,7 @@
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1">
         <v>200000</v>
@@ -2024,7 +2944,7 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1">
         <v>320000</v>

</xml_diff>